<commit_message>
Updates metadata for operations and adds in todos for other datasets
</commit_message>
<xml_diff>
--- a/data-raw/FISHBIO_submission/FISHBIO_PIT_Operations_metadata.xlsx
+++ b/data-raw/FISHBIO_submission/FISHBIO_PIT_Operations_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FISHBIO/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\data-stewardship\fishbio-stanislaus-o.mykiss\data-raw\FISHBIO_submission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47EBFA06-7858-DC46-B421-D0B2569607A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D2A3E4-49E0-43E9-BFD1-593ADA3D1566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29940" yWindow="-980" windowWidth="28800" windowHeight="17500" tabRatio="834" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="-15795" windowWidth="18960" windowHeight="13065" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>first_name</t>
   </si>
@@ -737,12 +737,12 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -753,7 +753,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -782,16 +782,16 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" customWidth="1"/>
-    <col min="10" max="10" width="32.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.375" customWidth="1"/>
+    <col min="10" max="10" width="32.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -838,29 +838,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMH10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F10:F12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="19.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.6640625" style="3"/>
-    <col min="3" max="3" width="13.1640625" style="12" customWidth="1"/>
+    <col min="1" max="2" width="19.625" style="3"/>
+    <col min="3" max="3" width="13.125" style="12" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="13.125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="5.375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="5.625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.125" style="12" customWidth="1"/>
     <col min="11" max="11" width="16" style="3" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="3" customWidth="1"/>
-    <col min="13" max="14" width="9.1640625" style="3" customWidth="1"/>
-    <col min="15" max="1022" width="19.6640625" style="3"/>
-    <col min="1023" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="12" max="12" width="17.625" style="3" customWidth="1"/>
+    <col min="13" max="14" width="9.125" style="3" customWidth="1"/>
+    <col min="15" max="1022" width="19.625" style="3"/>
+    <col min="1023" max="1025" width="8.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
@@ -904,7 +904,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>63</v>
       </c>
@@ -923,9 +923,14 @@
       <c r="L2" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="M2" s="7">
+        <v>44448</v>
+      </c>
+      <c r="N2" s="7">
+        <v>44684</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
@@ -939,16 +944,22 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H10" s="8"/>
     </row>
   </sheetData>
@@ -979,18 +990,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1001,7 +1012,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1016,14 +1027,14 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.875" customWidth="1"/>
+    <col min="5" max="5" width="27.375" customWidth="1"/>
     <col min="6" max="6" width="27" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1043,11 +1054,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="E3" s="1"/>
     </row>
@@ -1071,13 +1082,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="34.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1085,7 +1096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="115" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
     </row>
   </sheetData>
@@ -1102,13 +1113,13 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="46.625" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1116,7 +1127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1131,15 +1142,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.375" customWidth="1"/>
+    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1175,14 +1186,14 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9" style="9"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1221,17 +1232,17 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="21.625" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="9"/>
-    <col min="6" max="6" width="17.33203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="17.375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -1251,7 +1262,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -1279,12 +1290,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1318,17 +1329,17 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" customWidth="1"/>
-    <col min="8" max="8" width="53.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.125" customWidth="1"/>
+    <col min="2" max="2" width="23.875" customWidth="1"/>
+    <col min="3" max="3" width="22.625" customWidth="1"/>
+    <col min="4" max="4" width="24.125" customWidth="1"/>
+    <col min="5" max="5" width="23.875" customWidth="1"/>
+    <col min="8" max="8" width="53.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1351,27 +1362,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G8" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding info in weir operations metadata. Still not able to push to edi staging
</commit_message>
<xml_diff>
--- a/data-raw/FISHBIO_submission/FISHBIO_PIT_Operations_metadata.xlsx
+++ b/data-raw/FISHBIO_submission/FISHBIO_PIT_Operations_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\data-stewardship\fishbio-stanislaus-o.mykiss\data-raw\FISHBIO_submission\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/fishbio-stanislaus-o.mykiss/data-raw/FISHBIO_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D2A3E4-49E0-43E9-BFD1-593ADA3D1566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F16016E-A03C-3C49-B19B-F67BC6E58116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="-15795" windowWidth="18960" windowHeight="13065" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="attribute" sheetId="9" r:id="rId11"/>
     <sheet name="code_definitions" sheetId="10" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -227,15 +227,6 @@
     <t>tabular</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Operational Mode</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Date of operation action</t>
   </si>
   <si>
@@ -255,6 +246,15 @@
   </si>
   <si>
     <t>Comments describing nature of operation action</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>operation_mode</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
@@ -737,12 +737,12 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -753,7 +753,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -782,16 +782,16 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.625" customWidth="1"/>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="9" max="9" width="10.375" customWidth="1"/>
-    <col min="10" max="10" width="32.625" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -838,29 +838,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.625" style="3"/>
-    <col min="3" max="3" width="13.125" style="12" customWidth="1"/>
+    <col min="1" max="2" width="19.6640625" style="3"/>
+    <col min="3" max="3" width="13.1640625" style="12" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="13.125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="5.375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="5.625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" style="12" customWidth="1"/>
     <col min="11" max="11" width="16" style="3" customWidth="1"/>
-    <col min="12" max="12" width="17.625" style="3" customWidth="1"/>
-    <col min="13" max="14" width="9.125" style="3" customWidth="1"/>
-    <col min="15" max="1022" width="19.625" style="3"/>
-    <col min="1023" max="1025" width="8.375" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="3" customWidth="1"/>
+    <col min="13" max="14" width="9.1640625" style="3" customWidth="1"/>
+    <col min="15" max="1022" width="19.6640625" style="3"/>
+    <col min="1023" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
@@ -904,24 +904,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M2" s="7">
         <v>44448</v>
@@ -930,36 +930,36 @@
         <v>44684</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H10" s="8"/>
     </row>
   </sheetData>
@@ -994,14 +994,14 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1027,14 +1027,14 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
-    <col min="5" max="5" width="27.375" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
     <col min="6" max="6" width="27" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1054,11 +1054,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C3" s="1"/>
       <c r="E3" s="1"/>
     </row>
@@ -1082,13 +1082,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
-    <col min="2" max="2" width="34.875" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="115" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
     </row>
   </sheetData>
@@ -1113,13 +1113,13 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.625" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="46.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1142,15 +1142,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.375" customWidth="1"/>
-    <col min="2" max="2" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1186,14 +1186,14 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="9" style="9"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1232,17 +1232,17 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13.625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="21.625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="9"/>
-    <col min="6" max="6" width="17.375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -1290,12 +1290,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1329,17 +1329,17 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.125" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="3" max="3" width="22.625" customWidth="1"/>
-    <col min="4" max="4" width="24.125" customWidth="1"/>
-    <col min="5" max="5" width="23.875" customWidth="1"/>
-    <col min="8" max="8" width="53.625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="53.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1362,27 +1362,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G8" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates data on EDI, adding 2023 data
</commit_message>
<xml_diff>
--- a/data-raw/FISHBIO_submission/FISHBIO_PIT_Operations_metadata.xlsx
+++ b/data-raw/FISHBIO_submission/FISHBIO_PIT_Operations_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/fishbio-stanislaus-o.mykiss/data-raw/FISHBIO_submission/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erincain/Documents/Git/CVPIA/data-stewardship/fishbio-stanislaus-o.mykiss/data-raw/FISHBIO_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F16016E-A03C-3C49-B19B-F67BC6E58116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4735D4B0-A895-D844-8BA2-636D1C4956B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -251,10 +251,10 @@
     <t>date</t>
   </si>
   <si>
-    <t>operation_mode</t>
-  </si>
-  <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>operational_mode</t>
   </si>
 </sst>
 </file>
@@ -326,26 +326,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -435,7 +432,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -723,7 +720,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -839,20 +836,20 @@
   <dimension ref="A1:AMH10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="19.6640625" style="3"/>
-    <col min="3" max="3" width="13.1640625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="9" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="5.33203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="5.6640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="12.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" style="9" customWidth="1"/>
     <col min="11" max="11" width="16" style="3" customWidth="1"/>
     <col min="12" max="12" width="17.6640625" style="3" customWidth="1"/>
     <col min="13" max="14" width="9.1640625" style="3" customWidth="1"/>
@@ -867,7 +864,7 @@
       <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>55</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -888,7 +885,7 @@
       <c r="I1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="9" t="s">
         <v>47</v>
       </c>
       <c r="K1" s="3" t="s">
@@ -923,16 +920,16 @@
       <c r="L2" t="s">
         <v>65</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="6">
         <v>44448</v>
       </c>
-      <c r="N2" s="7">
+      <c r="N2" s="6">
         <v>44684</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>66</v>
@@ -946,7 +943,7 @@
     </row>
     <row r="4" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>69</v>
@@ -960,7 +957,7 @@
     </row>
     <row r="9" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="H10" s="8"/>
+      <c r="H10" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -1031,7 +1028,7 @@
   <cols>
     <col min="3" max="3" width="18.83203125" customWidth="1"/>
     <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27" style="9" customWidth="1"/>
+    <col min="6" max="6" width="27" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1050,7 +1047,7 @@
       <c r="E1" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1116,14 +1113,14 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1188,9 +1185,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="9" style="9"/>
+    <col min="3" max="3" width="9" style="8"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="9" style="9"/>
+    <col min="6" max="6" width="9" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1200,7 +1197,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -1209,7 +1206,7 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1235,40 +1232,40 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="8" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="9"/>
-    <col min="6" max="6" width="17.33203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="8"/>
+    <col min="6" max="6" width="17.33203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1363,27 +1360,27 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
+      <c r="A2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G3" s="7"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G4" s="7"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G5" s="7"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G6" s="7"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G7" s="7"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G8" s="7"/>
+      <c r="G8" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>